<commit_message>
Relatório de Custos  e Simulador
</commit_message>
<xml_diff>
--- a/Define/Relatório sobre custos..xlsx
+++ b/Define/Relatório sobre custos..xlsx
@@ -76,9 +76,6 @@
     <t>VOLUME DA PADS DIARIO</t>
   </si>
   <si>
-    <t>CUSTO POR HORA DO PAD</t>
-  </si>
-  <si>
     <t>CUSTO DE 1 DIA + ENERGIA + TELEFONE</t>
   </si>
   <si>
@@ -108,6 +105,9 @@
   <si>
     <t>CUSTO MÉDIO INDIRETO POR DIA
  PARA 1 SERVIDOR</t>
+  </si>
+  <si>
+    <t>CUSTO DE TRABALHO DE 1 SERVIDOR POR HORA NO PAD</t>
   </si>
 </sst>
 </file>
@@ -1558,8 +1558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1585,16 +1585,16 @@
         <v>7</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>25</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>0</v>
@@ -1641,7 +1641,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1">
         <v>431</v>
@@ -1651,13 +1651,13 @@
     </row>
     <row r="8" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
       <c r="D8" s="15"/>
       <c r="E8" s="27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G8" t="s">
         <v>9</v>
@@ -1710,7 +1710,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="28"/>
       <c r="C12" s="29"/>
@@ -1757,20 +1757,20 @@
       </c>
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
-      <c r="D19" s="13" t="e">
-        <f>B3+#REF!+D11</f>
-        <v>#REF!</v>
+      <c r="D19" s="13">
+        <f>B3+D12</f>
+        <v>14590.621846757263</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="11" t="e">
-        <f>D21*3</f>
-        <v>#REF!</v>
+      <c r="B20" s="28"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="11">
+        <f>D3*3</f>
+        <v>1450</v>
       </c>
       <c r="E20" s="10" t="s">
         <v>11</v>
@@ -1778,17 +1778,17 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
-      <c r="D21" s="8" t="e">
-        <f>D3+#REF!+#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E21" s="8" t="e">
+      <c r="D21" s="8">
+        <f>D3+E12</f>
+        <v>486.35406155857544</v>
+      </c>
+      <c r="E21" s="8">
         <f>D21*30</f>
-        <v>#REF!</v>
+        <v>14590.621846757263</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1819,9 +1819,9 @@
       </c>
       <c r="B24" s="14"/>
       <c r="C24" s="14"/>
-      <c r="D24" s="8" t="e">
+      <c r="D24" s="8">
         <f>D22*D19</f>
-        <v>#REF!</v>
+        <v>121588.51538964387</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1830,20 +1830,20 @@
       </c>
       <c r="B25" s="14"/>
       <c r="C25" s="14"/>
-      <c r="D25" s="8" t="e">
+      <c r="D25" s="8">
         <f>D21*D23</f>
-        <v>#REF!</v>
+        <v>135.09835043293762</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B26" s="14"/>
       <c r="C26" s="14"/>
-      <c r="D26" s="8" t="e">
+      <c r="D26" s="8">
         <f>D25/24</f>
-        <v>#REF!</v>
+        <v>5.6290979347057339</v>
       </c>
     </row>
   </sheetData>
@@ -1865,8 +1865,8 @@
     <mergeCell ref="A25:C25"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A18:F18"/>
+    <mergeCell ref="A20:C20"/>
     <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A20:C20"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>